<commit_message>
Representação de gráfico corrigida
</commit_message>
<xml_diff>
--- a/Informação de cidades.xlsx
+++ b/Informação de cidades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ATV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB44054-F010-4D1F-8927-85EC2A6F8DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969B85E0-BC05-4D35-8F6C-0ACAAD70F95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coordenadas" sheetId="1" r:id="rId1"/>
@@ -703,9 +703,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1045,18 +1046,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1067,120 +1070,130 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
+      <c r="D12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C12" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:C2 A6:A12 A3 A4 A5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2001,7 +2014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Condição de parada, mudança de constantes e gráfico de feromônios final
</commit_message>
<xml_diff>
--- a/Informação de cidades.xlsx
+++ b/Informação de cidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ATV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969B85E0-BC05-4D35-8F6C-0ACAAD70F95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA36014C-56A1-4F60-A9A4-FB01E1048A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,93 +40,33 @@
     <t>SANTOS</t>
   </si>
   <si>
-    <t>-23.96078</t>
-  </si>
-  <si>
-    <t>-46.33441</t>
-  </si>
-  <si>
     <t>CAMPINAS</t>
   </si>
   <si>
-    <t>-22.90551</t>
-  </si>
-  <si>
-    <t>-47.06112</t>
-  </si>
-  <si>
     <t>SOROCABA</t>
   </si>
   <si>
-    <t>-23.50070</t>
-  </si>
-  <si>
-    <t>-47.45796</t>
-  </si>
-  <si>
     <t>RIBEIRÃO PRETO</t>
   </si>
   <si>
-    <t>-21.17840</t>
-  </si>
-  <si>
-    <t>-47.80673</t>
-  </si>
-  <si>
     <t>ADAMANTINA</t>
   </si>
   <si>
-    <t>-21.68631</t>
-  </si>
-  <si>
-    <t>-51.07647</t>
-  </si>
-  <si>
     <t>SÃO JOSÉ DOS CAMPOS</t>
   </si>
   <si>
-    <t>-23.18588</t>
-  </si>
-  <si>
-    <t>-45.88662</t>
-  </si>
-  <si>
     <t>CAÇAPAVA</t>
   </si>
   <si>
-    <t>-23.09916</t>
-  </si>
-  <si>
-    <t>-45.70730</t>
-  </si>
-  <si>
     <t>AVARÉ</t>
   </si>
   <si>
-    <t>-23.10448</t>
-  </si>
-  <si>
-    <t>-48.92610</t>
-  </si>
-  <si>
     <t>AREIAS</t>
   </si>
   <si>
-    <t>-22.57977</t>
-  </si>
-  <si>
-    <t>-44.69761</t>
-  </si>
-  <si>
     <t>HOLAMBRA</t>
   </si>
   <si>
-    <t>-22.63320</t>
-  </si>
-  <si>
-    <t>-47.05453</t>
-  </si>
-  <si>
     <t>Distância entre cidades (em KM)</t>
   </si>
   <si>
@@ -668,14 +608,82 @@
   </si>
   <si>
     <t xml:space="preserve"> 83.60</t>
+  </si>
+  <si>
+    <t>23.96078</t>
+  </si>
+  <si>
+    <t>22.90551</t>
+  </si>
+  <si>
+    <t>23.50070</t>
+  </si>
+  <si>
+    <t>21.17840</t>
+  </si>
+  <si>
+    <t>21.68631</t>
+  </si>
+  <si>
+    <t>23.18588</t>
+  </si>
+  <si>
+    <t>23.09916</t>
+  </si>
+  <si>
+    <t>23.10448</t>
+  </si>
+  <si>
+    <t>22.57977</t>
+  </si>
+  <si>
+    <t>22.63320</t>
+  </si>
+  <si>
+    <t>47.05453</t>
+  </si>
+  <si>
+    <t>44.69761</t>
+  </si>
+  <si>
+    <t>48.92610</t>
+  </si>
+  <si>
+    <t>45.70730</t>
+  </si>
+  <si>
+    <t>45.88662</t>
+  </si>
+  <si>
+    <t>51.07647</t>
+  </si>
+  <si>
+    <t>47.80673</t>
+  </si>
+  <si>
+    <t>47.45796</t>
+  </si>
+  <si>
+    <t>47.06112</t>
+  </si>
+  <si>
+    <t>46.33441</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -703,10 +711,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1046,20 +1055,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1070,123 +1079,125 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B8" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B11" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>204</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>205</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -1208,7 +1219,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1219,31 +1230,31 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1251,349 +1262,349 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="J3" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="K3" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="K4" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
         <v>35</v>
       </c>
-      <c r="E5" t="s">
-        <v>55</v>
-      </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="I5" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="J5" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="K5" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="H6" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="I6" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="J6" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="K6" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="I7" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="J7" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="K7" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="I8" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="J8" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="K8" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="F9" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="G9" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="H9" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="I9" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="J9" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="K9" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="D10" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="G10" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="H10" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="I10" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="J10" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="K10" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="G11" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="H11" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="I11" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="J11" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="K11" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="G12" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="H12" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="I12" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="J12" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="K12" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1614,7 +1625,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1625,31 +1636,31 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1657,349 +1668,349 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="F3" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="G3" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="H3" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="I3" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="J3" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="K3" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="F4" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="G4" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="H4" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="I4" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="J4" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="K4" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" t="s">
         <v>106</v>
       </c>
-      <c r="E5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F5" t="s">
-        <v>126</v>
-      </c>
       <c r="G5" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="H5" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="I5" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="J5" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="K5" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" t="s">
+        <v>115</v>
+      </c>
+      <c r="I6" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" t="s">
         <v>117</v>
       </c>
-      <c r="D6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" t="s">
-        <v>133</v>
-      </c>
-      <c r="G6" t="s">
-        <v>134</v>
-      </c>
-      <c r="H6" t="s">
-        <v>135</v>
-      </c>
-      <c r="I6" t="s">
-        <v>136</v>
-      </c>
-      <c r="J6" t="s">
-        <v>137</v>
-      </c>
       <c r="K6" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E7" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="F7" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="G7" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="H7" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="I7" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="J7" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="K7" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="C8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" t="s">
         <v>119</v>
       </c>
-      <c r="D8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F8" t="s">
-        <v>139</v>
-      </c>
       <c r="G8" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="H8" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="I8" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="J8" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="K8" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="E9" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="F9" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="G9" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="H9" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="I9" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="J9" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="K9" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="E10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" t="s">
+        <v>124</v>
+      </c>
+      <c r="G10" t="s">
+        <v>131</v>
+      </c>
+      <c r="H10" t="s">
         <v>136</v>
       </c>
-      <c r="F10" t="s">
-        <v>144</v>
-      </c>
-      <c r="G10" t="s">
-        <v>151</v>
-      </c>
-      <c r="H10" t="s">
-        <v>156</v>
-      </c>
       <c r="I10" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="J10" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="K10" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="C11" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="D11" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="E11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" t="s">
+        <v>125</v>
+      </c>
+      <c r="G11" t="s">
+        <v>132</v>
+      </c>
+      <c r="H11" t="s">
         <v>137</v>
       </c>
-      <c r="F11" t="s">
-        <v>145</v>
-      </c>
-      <c r="G11" t="s">
-        <v>152</v>
-      </c>
-      <c r="H11" t="s">
-        <v>157</v>
-      </c>
       <c r="I11" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="J11" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="K11" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="E12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" t="s">
         <v>138</v>
       </c>
-      <c r="F12" t="s">
-        <v>146</v>
-      </c>
-      <c r="G12" t="s">
-        <v>153</v>
-      </c>
-      <c r="H12" t="s">
-        <v>158</v>
-      </c>
       <c r="I12" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="J12" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="K12" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2025,7 +2036,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2036,31 +2047,31 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2068,349 +2079,349 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="I7" s="1" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="G9" s="1">
         <v>10</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>